<commit_message>
Updated to start the mediaserver service on the UFT One host machine if it isn't running
</commit_message>
<xml_diff>
--- a/AI Cross Demo/Default.xlsx
+++ b/AI Cross Demo/Default.xlsx
@@ -283,10 +283,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
@@ -679,10 +679,10 @@
       <c s="2" t="b">
         <v>0</v>
       </c>
+      <c s="5" t="s">
+        <v>11</v>
+      </c>
       <c s="4" t="s">
-        <v>11</v>
-      </c>
-      <c s="5" t="s">
         <v>9</v>
       </c>
     </row>
@@ -703,10 +703,10 @@
       <c s="2" t="b">
         <v>0</v>
       </c>
+      <c s="5" t="s">
+        <v>11</v>
+      </c>
       <c s="4" t="s">
-        <v>11</v>
-      </c>
-      <c s="5" t="s">
         <v>9</v>
       </c>
     </row>
@@ -725,10 +725,10 @@
       <c s="2" t="b">
         <v>1</v>
       </c>
+      <c s="5" t="s">
+        <v>8</v>
+      </c>
       <c s="4" t="s">
-        <v>8</v>
-      </c>
-      <c s="5" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
made updates to not leverage autoscroll when not necessary
</commit_message>
<xml_diff>
--- a/AI Cross Demo/Default.xlsx
+++ b/AI Cross Demo/Default.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="24">
   <si>
     <t>Browser</t>
   </si>
@@ -26,10 +26,19 @@
     <t>CHROME</t>
   </si>
   <si>
+    <t>iPhone X</t>
+  </si>
+  <si>
+    <t>8e196b15f68b60004f89b0f745a52dcc45693309</t>
+  </si>
+  <si>
     <t>app_identifier</t>
   </si>
   <si>
-    <t>fd76a9d32fb7cc6eb6284cbcab936bc97dcfce35</t>
+    <t>Pixel 2</t>
+  </si>
+  <si>
+    <t>SAMSUNG-SM-G930A</t>
   </si>
   <si>
     <t>com.hpe.iShopping</t>
@@ -44,9 +53,6 @@
     <t>IOS</t>
   </si>
   <si>
-    <t>SM-G960F</t>
-  </si>
-  <si>
     <t>MC.Browser</t>
   </si>
   <si>
@@ -62,19 +68,19 @@
     <t>device_id</t>
   </si>
   <si>
-    <t>234c19cb26017ece</t>
-  </si>
-  <si>
     <t>ostype</t>
   </si>
   <si>
     <t>advantageonlineshopping.com/</t>
   </si>
   <si>
+    <t>2e8557b7</t>
+  </si>
+  <si>
     <t>com.Advantage.aShopping</t>
   </si>
   <si>
-    <t>iPhone 8</t>
+    <t>HT8641A00144</t>
   </si>
   <si>
     <t>URL</t>
@@ -283,13 +289,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -590,47 +596,47 @@
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView zoomScale="115" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="B1" zoomScale="115" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
     <col min="1" max="2" width="9.41796875" style="3" customWidth="1"/>
     <col min="3" max="3" width="32.76171875" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.15234375" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.57421875" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.3828125" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.359375" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.41796875" style="3" customWidth="1"/>
-    <col min="8" max="8" width="11.91015625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.8828125" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="16384" width="9.078125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row customFormat="1">
       <c t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c t="s">
         <v>0</v>
       </c>
       <c t="s">
-        <v>20</v>
+        <v>22</v>
+      </c>
+      <c t="s">
+        <v>16</v>
+      </c>
+      <c t="s">
+        <v>5</v>
+      </c>
+      <c t="s">
+        <v>15</v>
+      </c>
+      <c t="s">
+        <v>17</v>
       </c>
       <c t="s">
         <v>14</v>
       </c>
-      <c t="s">
-        <v>3</v>
-      </c>
-      <c t="s">
-        <v>13</v>
-      </c>
-      <c t="s">
-        <v>16</v>
-      </c>
-      <c t="s">
-        <v>12</v>
-      </c>
     </row>
     <row>
       <c s="1" t="s">
@@ -640,29 +646,29 @@
         <v>2</v>
       </c>
       <c s="1" t="s">
-        <v>21</v>
-      </c>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="6"/>
+        <v>23</v>
+      </c>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="4"/>
     </row>
     <row>
       <c s="1" t="s">
         <v>0</v>
       </c>
       <c s="1" t="s">
-        <v>7</v>
-      </c>
-      <c s="1" t="s">
-        <v>17</v>
-      </c>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="6"/>
+        <v>10</v>
+      </c>
+      <c s="1" t="s">
+        <v>18</v>
+      </c>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="4"/>
     </row>
     <row>
       <c s="1" t="s">
@@ -671,19 +677,41 @@
       <c s="1"/>
       <c s="1"/>
       <c s="2" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c s="2" t="s">
-        <v>18</v>
+        <v>8</v>
+      </c>
+      <c s="2" t="b">
+        <v>1</v>
+      </c>
+      <c s="5" t="s">
+        <v>11</v>
+      </c>
+      <c s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row>
+      <c s="1" t="s">
+        <v>1</v>
+      </c>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="2" t="s">
+        <v>19</v>
+      </c>
+      <c s="2" t="s">
+        <v>20</v>
       </c>
       <c s="2" t="b">
         <v>0</v>
       </c>
       <c s="5" t="s">
-        <v>11</v>
-      </c>
-      <c s="4" t="s">
-        <v>9</v>
+        <v>13</v>
+      </c>
+      <c s="6" t="s">
+        <v>7</v>
       </c>
     </row>
     <row>
@@ -692,44 +720,22 @@
       </c>
       <c s="1"/>
       <c s="1" t="s">
+        <v>23</v>
+      </c>
+      <c s="2" t="s">
         <v>21</v>
       </c>
       <c s="2" t="s">
-        <v>15</v>
-      </c>
-      <c s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c s="2" t="b">
         <v>0</v>
       </c>
       <c s="5" t="s">
-        <v>11</v>
-      </c>
-      <c s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row>
-      <c s="1" t="s">
-        <v>1</v>
-      </c>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="2" t="s">
-        <v>4</v>
-      </c>
-      <c s="2" t="s">
-        <v>5</v>
-      </c>
-      <c s="2" t="b">
-        <v>1</v>
-      </c>
-      <c s="5" t="s">
-        <v>8</v>
-      </c>
-      <c s="4" t="s">
-        <v>19</v>
+        <v>13</v>
+      </c>
+      <c s="6" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated to handle the occasional biometrics question that comes up on some devices sometimes.
</commit_message>
<xml_diff>
--- a/AI Cross Demo/Default.xlsx
+++ b/AI Cross Demo/Default.xlsx
@@ -289,13 +289,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -596,8 +596,8 @@
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="115" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView zoomScale="115" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
@@ -652,7 +652,7 @@
       <c s="1"/>
       <c s="1"/>
       <c s="1"/>
-      <c s="4"/>
+      <c s="6"/>
     </row>
     <row>
       <c s="1" t="s">
@@ -668,7 +668,7 @@
       <c s="1"/>
       <c s="1"/>
       <c s="1"/>
-      <c s="4"/>
+      <c s="6"/>
     </row>
     <row>
       <c s="1" t="s">
@@ -685,10 +685,10 @@
       <c s="2" t="b">
         <v>1</v>
       </c>
+      <c s="4" t="s">
+        <v>11</v>
+      </c>
       <c s="5" t="s">
-        <v>11</v>
-      </c>
-      <c s="6" t="s">
         <v>3</v>
       </c>
     </row>
@@ -707,10 +707,10 @@
       <c s="2" t="b">
         <v>0</v>
       </c>
+      <c s="4" t="s">
+        <v>13</v>
+      </c>
       <c s="5" t="s">
-        <v>13</v>
-      </c>
-      <c s="6" t="s">
         <v>7</v>
       </c>
     </row>
@@ -731,10 +731,10 @@
       <c s="2" t="b">
         <v>0</v>
       </c>
+      <c s="4" t="s">
+        <v>13</v>
+      </c>
       <c s="5" t="s">
-        <v>13</v>
-      </c>
-      <c s="6" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated the app_identifier data value in the data table for iOS to be com.mf.iShopping
</commit_message>
<xml_diff>
--- a/AI Cross Demo/Default.xlsx
+++ b/AI Cross Demo/Default.xlsx
@@ -41,7 +41,7 @@
     <t>SAMSUNG-SM-G930A</t>
   </si>
   <si>
-    <t>com.hpe.iShopping</t>
+    <t>com.mf.iShopping</t>
   </si>
   <si>
     <t>Context</t>
@@ -289,13 +289,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -596,7 +596,7 @@
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView zoomScale="115" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="115" workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -612,129 +612,129 @@
     <col min="9" max="16384" width="9.078125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1">
-      <c t="s">
+    <row r="1" ht="14.95" customFormat="1">
+      <c r="A1" t="s">
         <v>9</v>
       </c>
-      <c t="s">
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c t="s">
+      <c r="C1" t="s">
         <v>22</v>
       </c>
-      <c t="s">
+      <c r="D1" t="s">
         <v>16</v>
       </c>
-      <c t="s">
+      <c r="E1" t="s">
         <v>5</v>
       </c>
-      <c t="s">
+      <c r="F1" t="s">
         <v>15</v>
       </c>
-      <c t="s">
+      <c r="G1" t="s">
         <v>17</v>
       </c>
-      <c t="s">
+      <c r="H1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row>
-      <c s="1" t="s">
+    <row r="2">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>23</v>
       </c>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="6"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="5"/>
     </row>
-    <row>
-      <c s="1" t="s">
+    <row r="3">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>18</v>
       </c>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="6"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="5"/>
     </row>
-    <row>
-      <c s="1" t="s">
+    <row r="4">
+      <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="2" t="s">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="2" t="s">
         <v>4</v>
       </c>
-      <c s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>8</v>
       </c>
-      <c s="2" t="b">
+      <c r="F4" s="2" t="b">
         <v>1</v>
       </c>
-      <c s="4" t="s">
+      <c r="G4" s="6" t="s">
         <v>11</v>
       </c>
-      <c s="5" t="s">
+      <c r="H4" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row>
-      <c s="1" t="s">
+    <row r="5">
+      <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="2" t="s">
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="2" t="s">
         <v>19</v>
       </c>
-      <c s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>20</v>
       </c>
-      <c s="2" t="b">
+      <c r="F5" s="2" t="b">
         <v>0</v>
       </c>
-      <c s="4" t="s">
+      <c r="G5" s="6" t="s">
         <v>13</v>
       </c>
-      <c s="5" t="s">
+      <c r="H5" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row>
-      <c s="1" t="s">
+    <row r="6">
+      <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
-      <c s="1"/>
-      <c s="1" t="s">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1" t="s">
         <v>23</v>
       </c>
-      <c s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>21</v>
       </c>
-      <c s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>12</v>
       </c>
-      <c s="2" t="b">
+      <c r="F6" s="2" t="b">
         <v>0</v>
       </c>
-      <c s="4" t="s">
+      <c r="G6" s="6" t="s">
         <v>13</v>
       </c>
-      <c s="5" t="s">
+      <c r="H6" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -756,7 +756,7 @@
     <col min="1" max="16384" width="9.078125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1"/>
+    <row r="1" ht="14.95" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>